<commit_message>
Updated CAW Sheet for PM6 Purchases
</commit_message>
<xml_diff>
--- a/CAW Sheet/Team_2-4_CAW.xlsx
+++ b/CAW Sheet/Team_2-4_CAW.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\and1i\Desktop\Homework\Fall '23\ME EN 3230\Project\CAW Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75481F6-369E-4052-924C-4387ED926B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0950026-B797-4AB7-AF1B-7C07ECDAA4CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB16570C-9DD7-4F77-AE60-9DEA53993D96}"/>
+    <workbookView xWindow="8112" yWindow="2208" windowWidth="17280" windowHeight="8964" xr2:uid="{CB16570C-9DD7-4F77-AE60-9DEA53993D96}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
   <si>
     <t>Purchase Order and Budget</t>
   </si>
@@ -102,6 +102,51 @@
   </si>
   <si>
     <t>Alex Treseder</t>
+  </si>
+  <si>
+    <t>FS90 Servo</t>
+  </si>
+  <si>
+    <t>Limit Switch</t>
+  </si>
+  <si>
+    <t>Ball Castor Kit</t>
+  </si>
+  <si>
+    <t>84mm Wheels</t>
+  </si>
+  <si>
+    <t>GT2 Pulley 16T 5mm</t>
+  </si>
+  <si>
+    <t>Power Button</t>
+  </si>
+  <si>
+    <t>Antenna</t>
+  </si>
+  <si>
+    <t>Xbee</t>
+  </si>
+  <si>
+    <t>200mm Pulley Belt</t>
+  </si>
+  <si>
+    <t>400mm pulley belt</t>
+  </si>
+  <si>
+    <t>500mm Pulley Belt</t>
+  </si>
+  <si>
+    <t>20mm 78:1 Motor</t>
+  </si>
+  <si>
+    <t>L-Bracket for 37 mm Pololu motor</t>
+  </si>
+  <si>
+    <t>Pololu 20D mm Metal Gearmotor Bracket Pair</t>
+  </si>
+  <si>
+    <t>Wheel Hub Adapter for 6mm shaft</t>
   </si>
 </sst>
 </file>
@@ -150,7 +195,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -160,6 +205,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -245,7 +296,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -270,6 +321,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -286,10 +341,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -589,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E887DFA-1EA2-4ED9-ACEC-BE6D8ECCC88D}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="A6:G14"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="63" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -632,8 +683,8 @@
         <v>3</v>
       </c>
       <c r="G3" s="5">
-        <f>SUM(F6:F258)</f>
-        <v>184.03</v>
+        <f>SUM(F6:F257)</f>
+        <v>395.85</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -660,201 +711,553 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="6">
+      <c r="A6" s="14">
         <v>45189</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="15">
         <v>1</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="16">
         <v>21</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="16">
         <f>D6*E6</f>
         <v>21</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="15" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="6">
+      <c r="A7" s="14">
         <v>45189</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7" t="s">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="15">
         <v>1</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="16">
         <v>1.7</v>
       </c>
-      <c r="F7" s="8">
-        <f t="shared" ref="F7:F14" si="0">D7*E7</f>
+      <c r="F7" s="16">
+        <f t="shared" ref="F7:F30" si="0">D7*E7</f>
         <v>1.7</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="15" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="6">
+      <c r="A8" s="14">
         <v>45189</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7" t="s">
+      <c r="B8" s="15"/>
+      <c r="C8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="15">
         <v>1</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="16">
         <v>7.95</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="16">
         <f t="shared" si="0"/>
         <v>7.95</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="15" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="6">
+      <c r="A9" s="14">
         <v>45189</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7" t="s">
+      <c r="B9" s="15"/>
+      <c r="C9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="15">
         <v>1</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="16">
         <v>15.99</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="16">
         <f t="shared" si="0"/>
         <v>15.99</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="15" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="6">
+      <c r="A10" s="14">
         <v>45189</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7" t="s">
+      <c r="B10" s="15"/>
+      <c r="C10" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="15">
         <v>2</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="16">
         <v>16.989999999999998</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="16">
         <f t="shared" si="0"/>
         <v>33.979999999999997</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="15" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="6">
+      <c r="A11" s="14">
         <v>45190</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7" t="s">
+      <c r="B11" s="15"/>
+      <c r="C11" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="15">
         <v>1</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="16">
         <v>0.65</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="16">
         <f t="shared" si="0"/>
         <v>0.65</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="15" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="6">
+      <c r="A12" s="14">
         <v>45191</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="15">
         <v>1</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="16">
         <v>2.92</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="16">
         <f t="shared" si="0"/>
         <v>2.92</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="15" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="6">
+      <c r="A13" s="14">
         <v>45192</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7" t="s">
+      <c r="B13" s="15"/>
+      <c r="C13" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="15">
         <v>2</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="16">
         <v>47.79</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="16">
         <f t="shared" si="0"/>
         <v>95.58</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="15" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="6">
+      <c r="A14" s="14">
         <v>45193</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7" t="s">
+      <c r="B14" s="15"/>
+      <c r="C14" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="15">
         <v>1</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="16">
         <v>4.26</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="16">
         <f t="shared" si="0"/>
         <v>4.26</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="15" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="6">
+        <v>45198</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="7">
+        <v>2</v>
+      </c>
+      <c r="E15" s="7">
+        <v>8.42</v>
+      </c>
+      <c r="F15" s="8">
+        <f t="shared" si="0"/>
+        <v>16.84</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="6">
+        <v>45198</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="7">
+        <v>3</v>
+      </c>
+      <c r="E16" s="8">
+        <v>0.77</v>
+      </c>
+      <c r="F16" s="17">
+        <f t="shared" si="0"/>
+        <v>2.31</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="6">
+        <v>45198</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="7">
+        <v>1</v>
+      </c>
+      <c r="E17" s="8">
+        <v>3.19</v>
+      </c>
+      <c r="F17" s="17">
+        <f t="shared" si="0"/>
+        <v>3.19</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="6">
+        <v>45198</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="7">
+        <v>2</v>
+      </c>
+      <c r="E18" s="8">
+        <v>3.65</v>
+      </c>
+      <c r="F18" s="17">
+        <f t="shared" si="0"/>
+        <v>7.3</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="6">
+        <v>45198</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="7">
+        <v>4</v>
+      </c>
+      <c r="E19" s="8">
+        <v>1.47</v>
+      </c>
+      <c r="F19" s="17">
+        <f t="shared" si="0"/>
+        <v>5.88</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="6">
+        <v>45198</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="7">
+        <v>1</v>
+      </c>
+      <c r="E20" s="8">
+        <v>5.99</v>
+      </c>
+      <c r="F20" s="17">
+        <f t="shared" si="0"/>
+        <v>5.99</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="6">
+        <v>45198</v>
+      </c>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="7">
+        <v>1</v>
+      </c>
+      <c r="E21" s="8">
+        <v>1.36</v>
+      </c>
+      <c r="F21" s="17">
+        <f t="shared" si="0"/>
+        <v>1.36</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="6">
+        <v>45198</v>
+      </c>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="7">
+        <v>2</v>
+      </c>
+      <c r="E22" s="8">
+        <v>37.659999999999997</v>
+      </c>
+      <c r="F22" s="17">
+        <f t="shared" si="0"/>
+        <v>75.319999999999993</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="6">
+        <v>45198</v>
+      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="7">
+        <v>2</v>
+      </c>
+      <c r="E23" s="8">
+        <v>18.5</v>
+      </c>
+      <c r="F23" s="17">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="6">
+        <v>45198</v>
+      </c>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="7">
+        <v>2</v>
+      </c>
+      <c r="E24" s="8">
+        <v>5.47</v>
+      </c>
+      <c r="F24" s="17">
+        <f t="shared" si="0"/>
+        <v>10.94</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="6">
+        <v>45198</v>
+      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="7">
+        <v>1</v>
+      </c>
+      <c r="E25" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="F25" s="17">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="6">
+        <v>45198</v>
+      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="E26" s="8">
+        <v>2.52</v>
+      </c>
+      <c r="F26" s="17">
+        <f t="shared" si="0"/>
+        <v>1.26</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="6">
+        <v>45198</v>
+      </c>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="7">
+        <v>1</v>
+      </c>
+      <c r="E27" s="8">
+        <v>27.75</v>
+      </c>
+      <c r="F27" s="17">
+        <f t="shared" si="0"/>
+        <v>27.75</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="6">
+        <v>45198</v>
+      </c>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="7">
+        <v>1</v>
+      </c>
+      <c r="E28" s="8">
+        <v>7.31</v>
+      </c>
+      <c r="F28" s="17">
+        <f t="shared" si="0"/>
+        <v>7.31</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="6">
+        <v>45198</v>
+      </c>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="7">
+        <v>1</v>
+      </c>
+      <c r="E29" s="8">
+        <v>2.92</v>
+      </c>
+      <c r="F29" s="17">
+        <f t="shared" si="0"/>
+        <v>2.92</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="6">
+        <v>45198</v>
+      </c>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="7">
+        <v>1</v>
+      </c>
+      <c r="E30" s="8">
+        <v>4.95</v>
+      </c>
+      <c r="F30" s="17">
+        <f t="shared" si="0"/>
+        <v>4.95</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1039,18 +1442,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1073,14 +1476,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1F77AB8-A577-4754-ABC8-31302CAF9674}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7FC523A3-24FF-4287-82E4-B8830EE21F2A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -1095,4 +1490,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1F77AB8-A577-4754-ABC8-31302CAF9674}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
CAW Sheet added ABS plates
</commit_message>
<xml_diff>
--- a/CAW Sheet/Team_2-4_CAW.xlsx
+++ b/CAW Sheet/Team_2-4_CAW.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\and1i\Desktop\Homework\Fall '23\ME EN 3230\Project\CAW Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0950026-B797-4AB7-AF1B-7C07ECDAA4CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC519E6-1A43-4EE7-9371-8656C107F8EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8112" yWindow="2208" windowWidth="17280" windowHeight="8964" xr2:uid="{CB16570C-9DD7-4F77-AE60-9DEA53993D96}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB16570C-9DD7-4F77-AE60-9DEA53993D96}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
   <si>
     <t>Purchase Order and Budget</t>
   </si>
@@ -116,9 +116,6 @@
     <t>84mm Wheels</t>
   </si>
   <si>
-    <t>GT2 Pulley 16T 5mm</t>
-  </si>
-  <si>
     <t>Power Button</t>
   </si>
   <si>
@@ -132,9 +129,6 @@
   </si>
   <si>
     <t>400mm pulley belt</t>
-  </si>
-  <si>
-    <t>500mm Pulley Belt</t>
   </si>
   <si>
     <t>20mm 78:1 Motor</t>
@@ -296,7 +290,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -306,6 +300,9 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -321,10 +318,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -640,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E887DFA-1EA2-4ED9-ACEC-BE6D8ECCC88D}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="63" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScale="63" workbookViewId="0">
+      <selection activeCell="B29" sqref="A29:B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -656,15 +649,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="11"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -673,18 +666,18 @@
       <c r="B2" s="2">
         <v>2.4</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="16"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G3" s="5">
-        <f>SUM(F6:F257)</f>
-        <v>395.85</v>
+        <f>SUM(F6:F255)</f>
+        <v>289.17</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -711,200 +704,200 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="14">
+      <c r="A6" s="9">
         <v>45189</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15" t="s">
+      <c r="B6" s="10"/>
+      <c r="C6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="15">
-        <v>1</v>
-      </c>
-      <c r="E6" s="16">
+      <c r="D6" s="10">
+        <v>1</v>
+      </c>
+      <c r="E6" s="11">
         <v>21</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="11">
         <f>D6*E6</f>
         <v>21</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="14">
+      <c r="A7" s="9">
         <v>45189</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15" t="s">
+      <c r="B7" s="10"/>
+      <c r="C7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="15">
-        <v>1</v>
-      </c>
-      <c r="E7" s="16">
+      <c r="D7" s="10">
+        <v>1</v>
+      </c>
+      <c r="E7" s="11">
         <v>1.7</v>
       </c>
-      <c r="F7" s="16">
-        <f t="shared" ref="F7:F30" si="0">D7*E7</f>
+      <c r="F7" s="11">
+        <f t="shared" ref="F7:F29" si="0">D7*E7</f>
         <v>1.7</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="14">
+      <c r="A8" s="9">
         <v>45189</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15" t="s">
+      <c r="B8" s="10"/>
+      <c r="C8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="15">
-        <v>1</v>
-      </c>
-      <c r="E8" s="16">
+      <c r="D8" s="10">
+        <v>1</v>
+      </c>
+      <c r="E8" s="11">
         <v>7.95</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8" s="11">
         <f t="shared" si="0"/>
         <v>7.95</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="14">
+      <c r="A9" s="9">
         <v>45189</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15" t="s">
+      <c r="B9" s="10"/>
+      <c r="C9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="15">
-        <v>1</v>
-      </c>
-      <c r="E9" s="16">
+      <c r="D9" s="10">
+        <v>1</v>
+      </c>
+      <c r="E9" s="11">
         <v>15.99</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="11">
         <f t="shared" si="0"/>
         <v>15.99</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="14">
+      <c r="A10" s="9">
         <v>45189</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15" t="s">
+      <c r="B10" s="10"/>
+      <c r="C10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="10">
         <v>2</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="11">
         <v>16.989999999999998</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="11">
         <f t="shared" si="0"/>
         <v>33.979999999999997</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="14">
+      <c r="A11" s="9">
         <v>45190</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15" t="s">
+      <c r="B11" s="10"/>
+      <c r="C11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="15">
-        <v>1</v>
-      </c>
-      <c r="E11" s="16">
+      <c r="D11" s="10">
+        <v>1</v>
+      </c>
+      <c r="E11" s="11">
         <v>0.65</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F11" s="11">
         <f t="shared" si="0"/>
         <v>0.65</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="14">
+      <c r="A12" s="9">
         <v>45191</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15" t="s">
+      <c r="B12" s="10"/>
+      <c r="C12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="15">
-        <v>1</v>
-      </c>
-      <c r="E12" s="16">
+      <c r="D12" s="10">
+        <v>1</v>
+      </c>
+      <c r="E12" s="11">
         <v>2.92</v>
       </c>
-      <c r="F12" s="16">
+      <c r="F12" s="11">
         <f t="shared" si="0"/>
         <v>2.92</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="14">
+      <c r="A13" s="9">
         <v>45192</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15" t="s">
+      <c r="B13" s="10"/>
+      <c r="C13" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="10">
         <v>2</v>
       </c>
-      <c r="E13" s="16">
+      <c r="E13" s="11">
         <v>47.79</v>
       </c>
-      <c r="F13" s="16">
+      <c r="F13" s="11">
         <f t="shared" si="0"/>
         <v>95.58</v>
       </c>
-      <c r="G13" s="15" t="s">
+      <c r="G13" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="14">
+      <c r="A14" s="9">
         <v>45193</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15" t="s">
+      <c r="B14" s="10"/>
+      <c r="C14" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="15">
-        <v>1</v>
-      </c>
-      <c r="E14" s="16">
+      <c r="D14" s="10">
+        <v>1</v>
+      </c>
+      <c r="E14" s="11">
         <v>4.26</v>
       </c>
-      <c r="F14" s="16">
+      <c r="F14" s="11">
         <f t="shared" si="0"/>
         <v>4.26</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="10" t="s">
         <v>21</v>
       </c>
     </row>
@@ -914,7 +907,7 @@
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D15" s="7">
         <v>2</v>
@@ -944,7 +937,7 @@
       <c r="E16" s="8">
         <v>0.77</v>
       </c>
-      <c r="F16" s="17">
+      <c r="F16" s="8">
         <f t="shared" si="0"/>
         <v>2.31</v>
       </c>
@@ -966,7 +959,7 @@
       <c r="E17" s="8">
         <v>3.19</v>
       </c>
-      <c r="F17" s="17">
+      <c r="F17" s="8">
         <f t="shared" si="0"/>
         <v>3.19</v>
       </c>
@@ -988,7 +981,7 @@
       <c r="E18" s="8">
         <v>3.65</v>
       </c>
-      <c r="F18" s="17">
+      <c r="F18" s="8">
         <f t="shared" si="0"/>
         <v>7.3</v>
       </c>
@@ -1002,17 +995,17 @@
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D19" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E19" s="8">
-        <v>1.47</v>
-      </c>
-      <c r="F19" s="17">
-        <f t="shared" si="0"/>
-        <v>5.88</v>
+        <v>5.99</v>
+      </c>
+      <c r="F19" s="8">
+        <f t="shared" si="0"/>
+        <v>5.99</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>12</v>
@@ -1024,17 +1017,17 @@
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D20" s="7">
         <v>1</v>
       </c>
       <c r="E20" s="8">
-        <v>5.99</v>
-      </c>
-      <c r="F20" s="17">
-        <f t="shared" si="0"/>
-        <v>5.99</v>
+        <v>1.36</v>
+      </c>
+      <c r="F20" s="8">
+        <f t="shared" si="0"/>
+        <v>1.36</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>12</v>
@@ -1049,14 +1042,14 @@
         <v>27</v>
       </c>
       <c r="D21" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21" s="8">
-        <v>1.36</v>
-      </c>
-      <c r="F21" s="17">
-        <f t="shared" si="0"/>
-        <v>1.36</v>
+        <v>0</v>
+      </c>
+      <c r="F21" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>12</v>
@@ -1074,11 +1067,11 @@
         <v>2</v>
       </c>
       <c r="E22" s="8">
-        <v>37.659999999999997</v>
-      </c>
-      <c r="F22" s="17">
-        <f t="shared" si="0"/>
-        <v>75.319999999999993</v>
+        <v>0</v>
+      </c>
+      <c r="F22" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="G22" s="7" t="s">
         <v>12</v>
@@ -1090,17 +1083,17 @@
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="7" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D23" s="7">
         <v>2</v>
       </c>
       <c r="E23" s="8">
-        <v>18.5</v>
-      </c>
-      <c r="F23" s="17">
-        <f t="shared" si="0"/>
-        <v>37</v>
+        <v>5.47</v>
+      </c>
+      <c r="F23" s="8">
+        <f t="shared" si="0"/>
+        <v>10.94</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>12</v>
@@ -1112,17 +1105,17 @@
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D24" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E24" s="8">
-        <v>5.47</v>
-      </c>
-      <c r="F24" s="17">
-        <f t="shared" si="0"/>
-        <v>10.94</v>
+        <v>1.5</v>
+      </c>
+      <c r="F24" s="8">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
       </c>
       <c r="G24" s="7" t="s">
         <v>12</v>
@@ -1134,17 +1127,17 @@
       </c>
       <c r="B25" s="7"/>
       <c r="C25" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D25" s="7">
         <v>1</v>
       </c>
       <c r="E25" s="8">
-        <v>1.5</v>
-      </c>
-      <c r="F25" s="17">
-        <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>27.75</v>
+      </c>
+      <c r="F25" s="8">
+        <f t="shared" si="0"/>
+        <v>27.75</v>
       </c>
       <c r="G25" s="7" t="s">
         <v>12</v>
@@ -1156,17 +1149,17 @@
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D26" s="7">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E26" s="8">
-        <v>2.52</v>
-      </c>
-      <c r="F26" s="17">
-        <f t="shared" si="0"/>
-        <v>1.26</v>
+        <v>7.31</v>
+      </c>
+      <c r="F26" s="8">
+        <f t="shared" si="0"/>
+        <v>7.31</v>
       </c>
       <c r="G26" s="7" t="s">
         <v>12</v>
@@ -1178,17 +1171,17 @@
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="7" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="D27" s="7">
         <v>1</v>
       </c>
       <c r="E27" s="8">
-        <v>27.75</v>
-      </c>
-      <c r="F27" s="17">
-        <f t="shared" si="0"/>
-        <v>27.75</v>
+        <v>2.92</v>
+      </c>
+      <c r="F27" s="8">
+        <f t="shared" si="0"/>
+        <v>2.92</v>
       </c>
       <c r="G27" s="7" t="s">
         <v>12</v>
@@ -1200,17 +1193,17 @@
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="7" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="D28" s="7">
         <v>1</v>
       </c>
       <c r="E28" s="8">
-        <v>7.31</v>
-      </c>
-      <c r="F28" s="17">
-        <f t="shared" si="0"/>
-        <v>7.31</v>
+        <v>4.95</v>
+      </c>
+      <c r="F28" s="8">
+        <f t="shared" si="0"/>
+        <v>4.95</v>
       </c>
       <c r="G28" s="7" t="s">
         <v>12</v>
@@ -1222,41 +1215,19 @@
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D29" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E29" s="8">
-        <v>2.92</v>
-      </c>
-      <c r="F29" s="17">
-        <f t="shared" si="0"/>
-        <v>2.92</v>
+        <v>4.26</v>
+      </c>
+      <c r="F29" s="8">
+        <f t="shared" si="0"/>
+        <v>12.78</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="6">
-        <v>45198</v>
-      </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D30" s="7">
-        <v>1</v>
-      </c>
-      <c r="E30" s="8">
-        <v>4.95</v>
-      </c>
-      <c r="F30" s="17">
-        <f t="shared" si="0"/>
-        <v>4.95</v>
-      </c>
-      <c r="G30" s="7" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1271,6 +1242,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011AD271953E1094AB74D69C72394D954" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="be1910e1736fcdcd817e8ca87c829ba5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="873979c6-3d0f-404b-99e3-69e94fedc1c2" xmlns:ns4="63bea315-07aa-4f33-8ec6-dda8e4efdc3e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4480402d69e31faf1fded5495ec700ba" ns3:_="" ns4:_="">
     <xsd:import namespace="873979c6-3d0f-404b-99e3-69e94fedc1c2"/>
@@ -1441,36 +1427,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1064D0D-C90A-4277-BB8B-150D7DAAE2C4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1F77AB8-A577-4754-ABC8-31302CAF9674}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="873979c6-3d0f-404b-99e3-69e94fedc1c2"/>
-    <ds:schemaRef ds:uri="63bea315-07aa-4f33-8ec6-dda8e4efdc3e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1493,9 +1453,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1F77AB8-A577-4754-ABC8-31302CAF9674}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1064D0D-C90A-4277-BB8B-150D7DAAE2C4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="873979c6-3d0f-404b-99e3-69e94fedc1c2"/>
+    <ds:schemaRef ds:uri="63bea315-07aa-4f33-8ec6-dda8e4efdc3e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Post PS6 update. Code working.
</commit_message>
<xml_diff>
--- a/CAW Sheet/Team_2-4_CAW.xlsx
+++ b/CAW Sheet/Team_2-4_CAW.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\and1i\Desktop\Homework\Fall '23\ME EN 3230\Project\CAW Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC519E6-1A43-4EE7-9371-8656C107F8EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1942A9E-97D1-4B32-BCEF-FF71F90565BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB16570C-9DD7-4F77-AE60-9DEA53993D96}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="36">
   <si>
     <t>Purchase Order and Budget</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>Wheel Hub Adapter for 6mm shaft</t>
+  </si>
+  <si>
+    <t>Battery Connector</t>
   </si>
 </sst>
 </file>
@@ -189,18 +192,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -290,7 +287,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -300,9 +297,6 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -318,6 +312,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -633,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E887DFA-1EA2-4ED9-ACEC-BE6D8ECCC88D}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="63" workbookViewId="0">
-      <selection activeCell="B29" sqref="A29:B29"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="86" workbookViewId="0">
+      <selection activeCell="G17" sqref="A17:G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -649,15 +644,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="14"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -666,10 +661,10 @@
       <c r="B2" s="2">
         <v>2.4</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="16"/>
+      <c r="G2" s="13"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F3" s="4" t="s">
@@ -677,7 +672,7 @@
       </c>
       <c r="G3" s="5">
         <f>SUM(F6:F255)</f>
-        <v>289.17</v>
+        <v>292.76</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -704,200 +699,200 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="9">
+      <c r="A6" s="6">
         <v>45189</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10" t="s">
+      <c r="B6" s="7"/>
+      <c r="C6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="10">
-        <v>1</v>
-      </c>
-      <c r="E6" s="11">
+      <c r="D6" s="7">
+        <v>1</v>
+      </c>
+      <c r="E6" s="8">
         <v>21</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="8">
         <f>D6*E6</f>
         <v>21</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="9">
+      <c r="A7" s="6">
         <v>45189</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10" t="s">
+      <c r="B7" s="7"/>
+      <c r="C7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="10">
-        <v>1</v>
-      </c>
-      <c r="E7" s="11">
+      <c r="D7" s="7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="8">
         <v>1.7</v>
       </c>
-      <c r="F7" s="11">
-        <f t="shared" ref="F7:F29" si="0">D7*E7</f>
+      <c r="F7" s="8">
+        <f t="shared" ref="F7:F31" si="0">D7*E7</f>
         <v>1.7</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="9">
+      <c r="A8" s="6">
         <v>45189</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10" t="s">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="10">
-        <v>1</v>
-      </c>
-      <c r="E8" s="11">
+      <c r="D8" s="7">
+        <v>1</v>
+      </c>
+      <c r="E8" s="8">
         <v>7.95</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="8">
         <f t="shared" si="0"/>
         <v>7.95</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="9">
+      <c r="A9" s="6">
         <v>45189</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10" t="s">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="10">
-        <v>1</v>
-      </c>
-      <c r="E9" s="11">
+      <c r="D9" s="7">
+        <v>1</v>
+      </c>
+      <c r="E9" s="8">
         <v>15.99</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="8">
         <f t="shared" si="0"/>
         <v>15.99</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="9">
+      <c r="A10" s="6">
         <v>45189</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10" t="s">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="7">
         <v>2</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="8">
         <v>16.989999999999998</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="8">
         <f t="shared" si="0"/>
         <v>33.979999999999997</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="9">
+      <c r="A11" s="6">
         <v>45190</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10" t="s">
+      <c r="B11" s="7"/>
+      <c r="C11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="10">
-        <v>1</v>
-      </c>
-      <c r="E11" s="11">
+      <c r="D11" s="7">
+        <v>1</v>
+      </c>
+      <c r="E11" s="8">
         <v>0.65</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="8">
         <f t="shared" si="0"/>
         <v>0.65</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="9">
+      <c r="A12" s="6">
         <v>45191</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10" t="s">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="10">
-        <v>1</v>
-      </c>
-      <c r="E12" s="11">
+      <c r="D12" s="7">
+        <v>1</v>
+      </c>
+      <c r="E12" s="8">
         <v>2.92</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="8">
         <f t="shared" si="0"/>
         <v>2.92</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="9">
+      <c r="A13" s="6">
         <v>45192</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10" t="s">
+      <c r="B13" s="7"/>
+      <c r="C13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="7">
         <v>2</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="8">
         <v>47.79</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="8">
         <f t="shared" si="0"/>
         <v>95.58</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="9">
+      <c r="A14" s="6">
         <v>45193</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10" t="s">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="10">
-        <v>1</v>
-      </c>
-      <c r="E14" s="11">
+      <c r="D14" s="7">
+        <v>1</v>
+      </c>
+      <c r="E14" s="8">
         <v>4.26</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="8">
         <f t="shared" si="0"/>
         <v>4.26</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="7" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1228,6 +1223,48 @@
         <v>12.78</v>
       </c>
       <c r="G29" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="14">
+        <v>45202</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" s="7">
+        <v>1</v>
+      </c>
+      <c r="E30" s="8">
+        <v>3.19</v>
+      </c>
+      <c r="F30" s="8">
+        <f t="shared" si="0"/>
+        <v>3.19</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="14">
+        <v>45202</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" s="7">
+        <v>1</v>
+      </c>
+      <c r="E31" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="F31" s="8">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="G31" s="7" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated code and CAW sheet for Fall Break.
</commit_message>
<xml_diff>
--- a/CAW Sheet/Team_2-4_CAW.xlsx
+++ b/CAW Sheet/Team_2-4_CAW.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\and1i\Desktop\Homework\Fall '23\ME EN 3230\Project\CAW Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1942A9E-97D1-4B32-BCEF-FF71F90565BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E3790F-6E6B-4DE3-B40E-875D5CEDBD78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB16570C-9DD7-4F77-AE60-9DEA53993D96}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="39">
   <si>
     <t>Purchase Order and Budget</t>
   </si>
@@ -144,6 +144,15 @@
   </si>
   <si>
     <t>Battery Connector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distance Sensor - GP2Y0A51SK0F </t>
+  </si>
+  <si>
+    <t>3-Pin D.S. Cable for 2-15cm</t>
+  </si>
+  <si>
+    <t>Reflectance Array - QTR-HD-13</t>
   </si>
 </sst>
 </file>
@@ -153,7 +162,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,8 +200,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -202,6 +223,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -287,7 +314,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -297,6 +324,7 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -312,7 +340,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -628,10 +661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E887DFA-1EA2-4ED9-ACEC-BE6D8ECCC88D}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="86" workbookViewId="0">
-      <selection activeCell="G17" sqref="A17:G31"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -644,15 +677,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="11"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -661,18 +694,18 @@
       <c r="B2" s="2">
         <v>2.4</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="13"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G3" s="5">
-        <f>SUM(F6:F255)</f>
-        <v>292.76</v>
+        <f>SUM(F6:F254)</f>
+        <v>324.99</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -735,7 +768,7 @@
         <v>1.7</v>
       </c>
       <c r="F7" s="8">
-        <f t="shared" ref="F7:F31" si="0">D7*E7</f>
+        <f t="shared" ref="F7:F34" si="0">D7*E7</f>
         <v>1.7</v>
       </c>
       <c r="G7" s="7" t="s">
@@ -1227,7 +1260,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="14">
+      <c r="A30" s="9">
         <v>45202</v>
       </c>
       <c r="C30" s="7" t="s">
@@ -1248,7 +1281,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="14">
+      <c r="A31" s="9">
         <v>45202</v>
       </c>
       <c r="C31" s="7" t="s">
@@ -1267,6 +1300,75 @@
       <c r="G31" s="7" t="s">
         <v>12</v>
       </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="15">
+        <v>45209</v>
+      </c>
+      <c r="B32" s="16"/>
+      <c r="C32" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" s="16">
+        <v>1</v>
+      </c>
+      <c r="E32" s="18">
+        <v>20.41</v>
+      </c>
+      <c r="F32" s="19">
+        <f t="shared" si="0"/>
+        <v>20.41</v>
+      </c>
+      <c r="G32" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="15">
+        <v>45209</v>
+      </c>
+      <c r="B33" s="16"/>
+      <c r="C33" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" s="16">
+        <v>1</v>
+      </c>
+      <c r="E33" s="18">
+        <v>10.56</v>
+      </c>
+      <c r="F33" s="19">
+        <f t="shared" si="0"/>
+        <v>10.56</v>
+      </c>
+      <c r="G33" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="15">
+        <v>45209</v>
+      </c>
+      <c r="B34" s="16"/>
+      <c r="C34" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" s="16">
+        <v>1</v>
+      </c>
+      <c r="E34" s="18">
+        <v>1.26</v>
+      </c>
+      <c r="F34" s="19">
+        <f t="shared" si="0"/>
+        <v>1.26</v>
+      </c>
+      <c r="G34" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C35" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1279,21 +1381,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011AD271953E1094AB74D69C72394D954" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="be1910e1736fcdcd817e8ca87c829ba5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="873979c6-3d0f-404b-99e3-69e94fedc1c2" xmlns:ns4="63bea315-07aa-4f33-8ec6-dda8e4efdc3e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4480402d69e31faf1fded5495ec700ba" ns3:_="" ns4:_="">
     <xsd:import namespace="873979c6-3d0f-404b-99e3-69e94fedc1c2"/>
@@ -1464,10 +1551,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1F77AB8-A577-4754-ABC8-31302CAF9674}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1064D0D-C90A-4277-BB8B-150D7DAAE2C4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="873979c6-3d0f-404b-99e3-69e94fedc1c2"/>
+    <ds:schemaRef ds:uri="63bea315-07aa-4f33-8ec6-dda8e4efdc3e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1490,20 +1603,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1064D0D-C90A-4277-BB8B-150D7DAAE2C4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1F77AB8-A577-4754-ABC8-31302CAF9674}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="873979c6-3d0f-404b-99e3-69e94fedc1c2"/>
-    <ds:schemaRef ds:uri="63bea315-07aa-4f33-8ec6-dda8e4efdc3e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
October 27 PM8 Update
</commit_message>
<xml_diff>
--- a/CAW Sheet/Team_2-4_CAW.xlsx
+++ b/CAW Sheet/Team_2-4_CAW.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\and1i\Desktop\Homework\Fall '23\ME EN 3230\Project\CAW Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E3790F-6E6B-4DE3-B40E-875D5CEDBD78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BD66C2-0519-4A80-8313-7832C0EF1598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB16570C-9DD7-4F77-AE60-9DEA53993D96}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="43">
   <si>
     <t>Purchase Order and Budget</t>
   </si>
@@ -153,6 +153,18 @@
   </si>
   <si>
     <t>Reflectance Array - QTR-HD-13</t>
+  </si>
+  <si>
+    <t>Power Servo 3001HB</t>
+  </si>
+  <si>
+    <t>Buck Converters</t>
+  </si>
+  <si>
+    <t>Distance Sensor GP2Y0A41SK0F 4-30 cm</t>
+  </si>
+  <si>
+    <t>p;</t>
   </si>
 </sst>
 </file>
@@ -325,6 +337,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -340,12 +356,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -661,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E887DFA-1EA2-4ED9-ACEC-BE6D8ECCC88D}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="86" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="86" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -677,15 +689,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="12"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="16"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -694,10 +706,10 @@
       <c r="B2" s="2">
         <v>2.4</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="18"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F3" s="4" t="s">
@@ -705,7 +717,7 @@
       </c>
       <c r="G3" s="5">
         <f>SUM(F6:F254)</f>
-        <v>324.99</v>
+        <v>384.79</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -768,7 +780,7 @@
         <v>1.7</v>
       </c>
       <c r="F7" s="8">
-        <f t="shared" ref="F7:F34" si="0">D7*E7</f>
+        <f t="shared" ref="F7:F38" si="0">D7*E7</f>
         <v>1.7</v>
       </c>
       <c r="G7" s="7" t="s">
@@ -973,7 +985,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>45198</v>
       </c>
@@ -995,7 +1007,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>45198</v>
       </c>
@@ -1017,7 +1029,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>45198</v>
       </c>
@@ -1039,7 +1051,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>45198</v>
       </c>
@@ -1061,7 +1073,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>45198</v>
       </c>
@@ -1083,7 +1095,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>45198</v>
       </c>
@@ -1105,7 +1117,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>45198</v>
       </c>
@@ -1127,7 +1139,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>45198</v>
       </c>
@@ -1149,7 +1161,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>45198</v>
       </c>
@@ -1171,7 +1183,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>45198</v>
       </c>
@@ -1193,7 +1205,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>45198</v>
       </c>
@@ -1215,7 +1227,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>45198</v>
       </c>
@@ -1237,7 +1249,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>45198</v>
       </c>
@@ -1259,7 +1271,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="9">
         <v>45202</v>
       </c>
@@ -1280,7 +1292,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="9">
         <v>45202</v>
       </c>
@@ -1301,74 +1313,162 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="15">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="6">
         <v>45209</v>
       </c>
-      <c r="B32" s="16"/>
-      <c r="C32" s="16" t="s">
+      <c r="B32" s="7"/>
+      <c r="C32" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="16">
-        <v>1</v>
-      </c>
-      <c r="E32" s="18">
+      <c r="D32" s="7">
+        <v>1</v>
+      </c>
+      <c r="E32" s="8">
         <v>20.41</v>
       </c>
-      <c r="F32" s="19">
+      <c r="F32" s="8">
         <f t="shared" si="0"/>
         <v>20.41</v>
       </c>
-      <c r="G32" s="16" t="s">
-        <v>12</v>
+      <c r="G32" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H32" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="15">
+      <c r="A33" s="6">
         <v>45209</v>
       </c>
-      <c r="B33" s="16"/>
-      <c r="C33" s="16" t="s">
+      <c r="B33" s="7"/>
+      <c r="C33" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D33" s="16">
-        <v>1</v>
-      </c>
-      <c r="E33" s="18">
+      <c r="D33" s="7">
+        <v>1</v>
+      </c>
+      <c r="E33" s="8">
         <v>10.56</v>
       </c>
-      <c r="F33" s="19">
+      <c r="F33" s="8">
         <f t="shared" si="0"/>
         <v>10.56</v>
       </c>
-      <c r="G33" s="16" t="s">
+      <c r="G33" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="15">
+      <c r="A34" s="6">
         <v>45209</v>
       </c>
-      <c r="B34" s="16"/>
-      <c r="C34" s="17" t="s">
+      <c r="B34" s="7"/>
+      <c r="C34" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="D34" s="16">
-        <v>1</v>
-      </c>
-      <c r="E34" s="18">
+      <c r="D34" s="7">
+        <v>1</v>
+      </c>
+      <c r="E34" s="8">
         <v>1.26</v>
       </c>
-      <c r="F34" s="19">
+      <c r="F34" s="8">
         <f t="shared" si="0"/>
         <v>1.26</v>
       </c>
-      <c r="G34" s="16" t="s">
+      <c r="G34" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C35" s="20"/>
+      <c r="A35" s="10">
+        <v>45225</v>
+      </c>
+      <c r="B35" s="11"/>
+      <c r="C35" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" s="11">
+        <v>5</v>
+      </c>
+      <c r="E35" s="13">
+        <v>4.26</v>
+      </c>
+      <c r="F35" s="13">
+        <f t="shared" si="0"/>
+        <v>21.299999999999997</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="10">
+        <v>45225</v>
+      </c>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" s="11">
+        <v>2</v>
+      </c>
+      <c r="E36" s="13">
+        <v>12.17</v>
+      </c>
+      <c r="F36" s="13">
+        <f t="shared" si="0"/>
+        <v>24.34</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="10">
+        <v>45225</v>
+      </c>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" s="11">
+        <v>2</v>
+      </c>
+      <c r="E37" s="13">
+        <v>1.8</v>
+      </c>
+      <c r="F37" s="13">
+        <f t="shared" si="0"/>
+        <v>3.6</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="10">
+        <v>45225</v>
+      </c>
+      <c r="B38" s="11"/>
+      <c r="C38" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38" s="11">
+        <v>1</v>
+      </c>
+      <c r="E38" s="13">
+        <v>10.56</v>
+      </c>
+      <c r="F38" s="13">
+        <f t="shared" si="0"/>
+        <v>10.56</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1381,6 +1481,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011AD271953E1094AB74D69C72394D954" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="be1910e1736fcdcd817e8ca87c829ba5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="873979c6-3d0f-404b-99e3-69e94fedc1c2" xmlns:ns4="63bea315-07aa-4f33-8ec6-dda8e4efdc3e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4480402d69e31faf1fded5495ec700ba" ns3:_="" ns4:_="">
     <xsd:import namespace="873979c6-3d0f-404b-99e3-69e94fedc1c2"/>
@@ -1551,36 +1666,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1064D0D-C90A-4277-BB8B-150D7DAAE2C4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1F77AB8-A577-4754-ABC8-31302CAF9674}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="873979c6-3d0f-404b-99e3-69e94fedc1c2"/>
-    <ds:schemaRef ds:uri="63bea315-07aa-4f33-8ec6-dda8e4efdc3e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1603,9 +1692,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1F77AB8-A577-4754-ABC8-31302CAF9674}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1064D0D-C90A-4277-BB8B-150D7DAAE2C4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="873979c6-3d0f-404b-99e3-69e94fedc1c2"/>
+    <ds:schemaRef ds:uri="63bea315-07aa-4f33-8ec6-dda8e4efdc3e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated code for PM10
</commit_message>
<xml_diff>
--- a/CAW Sheet/Team_2-4_CAW.xlsx
+++ b/CAW Sheet/Team_2-4_CAW.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\and1i\Desktop\Homework\Fall '23\ME EN 3230\Project\CAW Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BD66C2-0519-4A80-8313-7832C0EF1598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E0E73E-3BF8-4810-9430-9EF8EAB02E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB16570C-9DD7-4F77-AE60-9DEA53993D96}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="46">
   <si>
     <t>Purchase Order and Budget</t>
   </si>
@@ -165,6 +165,15 @@
   </si>
   <si>
     <t>p;</t>
+  </si>
+  <si>
+    <t>GT2 4mm bore, 20-tooth pulley</t>
+  </si>
+  <si>
+    <t>200mm GT2 Timing Belt</t>
+  </si>
+  <si>
+    <t>GT2 5mm bore, 20-tooth pulley</t>
   </si>
 </sst>
 </file>
@@ -326,7 +335,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -339,8 +348,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -356,8 +366,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -673,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E887DFA-1EA2-4ED9-ACEC-BE6D8ECCC88D}">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="86" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="86" workbookViewId="0">
+      <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -689,15 +697,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="16"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -706,10 +714,10 @@
       <c r="B2" s="2">
         <v>2.4</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="18"/>
+      <c r="G2" s="19"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F3" s="4" t="s">
@@ -717,7 +725,7 @@
       </c>
       <c r="G3" s="5">
         <f>SUM(F6:F254)</f>
-        <v>384.79</v>
+        <v>389.89000000000004</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -780,7 +788,7 @@
         <v>1.7</v>
       </c>
       <c r="F7" s="8">
-        <f t="shared" ref="F7:F38" si="0">D7*E7</f>
+        <f t="shared" ref="F7:F40" si="0">D7*E7</f>
         <v>1.7</v>
       </c>
       <c r="G7" s="7" t="s">
@@ -1365,7 +1373,7 @@
         <v>45209</v>
       </c>
       <c r="B34" s="7"/>
-      <c r="C34" s="19" t="s">
+      <c r="C34" s="13" t="s">
         <v>37</v>
       </c>
       <c r="D34" s="7">
@@ -1383,90 +1391,178 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="10">
+      <c r="A35" s="6">
         <v>45225</v>
       </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="20" t="s">
+      <c r="B35" s="7"/>
+      <c r="C35" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D35" s="11">
+      <c r="D35" s="7">
         <v>5</v>
       </c>
-      <c r="E35" s="13">
+      <c r="E35" s="8">
         <v>4.26</v>
       </c>
-      <c r="F35" s="13">
+      <c r="F35" s="8">
         <f t="shared" si="0"/>
         <v>21.299999999999997</v>
       </c>
-      <c r="G35" s="11" t="s">
+      <c r="G35" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="10">
+      <c r="A36" s="6">
         <v>45225</v>
       </c>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11" t="s">
+      <c r="B36" s="7"/>
+      <c r="C36" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D36" s="11">
+      <c r="D36" s="7">
         <v>2</v>
       </c>
-      <c r="E36" s="13">
+      <c r="E36" s="8">
         <v>12.17</v>
       </c>
-      <c r="F36" s="13">
+      <c r="F36" s="8">
         <f t="shared" si="0"/>
         <v>24.34</v>
       </c>
-      <c r="G36" s="11" t="s">
+      <c r="G36" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="10">
+      <c r="A37" s="6">
         <v>45225</v>
       </c>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11" t="s">
+      <c r="B37" s="7"/>
+      <c r="C37" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D37" s="11">
+      <c r="D37" s="7">
         <v>2</v>
       </c>
-      <c r="E37" s="13">
+      <c r="E37" s="8">
         <v>1.8</v>
       </c>
-      <c r="F37" s="13">
+      <c r="F37" s="8">
         <f t="shared" si="0"/>
         <v>3.6</v>
       </c>
-      <c r="G37" s="11" t="s">
+      <c r="G37" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="10">
+      <c r="A38" s="6">
         <v>45225</v>
       </c>
-      <c r="B38" s="11"/>
-      <c r="C38" s="12" t="s">
+      <c r="B38" s="7"/>
+      <c r="C38" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D38" s="11">
-        <v>1</v>
-      </c>
-      <c r="E38" s="13">
+      <c r="D38" s="7">
+        <v>1</v>
+      </c>
+      <c r="E38" s="8">
         <v>10.56</v>
       </c>
-      <c r="F38" s="13">
+      <c r="F38" s="8">
         <f t="shared" si="0"/>
         <v>10.56</v>
       </c>
-      <c r="G38" s="11" t="s">
+      <c r="G38" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="6">
+        <v>45231</v>
+      </c>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D39" s="7">
+        <v>2</v>
+      </c>
+      <c r="E39" s="8">
+        <v>2.12</v>
+      </c>
+      <c r="F39" s="8">
+        <f t="shared" si="0"/>
+        <v>4.24</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="6">
+        <v>45231</v>
+      </c>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D40" s="7">
+        <v>1</v>
+      </c>
+      <c r="E40" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="F40" s="8">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="10">
+        <v>45231</v>
+      </c>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D41" s="11">
+        <v>2</v>
+      </c>
+      <c r="E41" s="12">
+        <v>1.8</v>
+      </c>
+      <c r="F41" s="12">
+        <f t="shared" ref="F41:F42" si="1">D41*E41</f>
+        <v>3.6</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="10">
+        <v>45231</v>
+      </c>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D42" s="11">
+        <v>2</v>
+      </c>
+      <c r="E42" s="12">
+        <v>-2.12</v>
+      </c>
+      <c r="F42" s="12">
+        <f t="shared" si="1"/>
+        <v>-4.24</v>
+      </c>
+      <c r="G42" s="11" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1481,21 +1577,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011AD271953E1094AB74D69C72394D954" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="be1910e1736fcdcd817e8ca87c829ba5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="873979c6-3d0f-404b-99e3-69e94fedc1c2" xmlns:ns4="63bea315-07aa-4f33-8ec6-dda8e4efdc3e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4480402d69e31faf1fded5495ec700ba" ns3:_="" ns4:_="">
     <xsd:import namespace="873979c6-3d0f-404b-99e3-69e94fedc1c2"/>
@@ -1666,15 +1753,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1F77AB8-A577-4754-ABC8-31302CAF9674}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7FC523A3-24FF-4287-82E4-B8830EE21F2A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -1691,7 +1779,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1064D0D-C90A-4277-BB8B-150D7DAAE2C4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1708,4 +1796,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1F77AB8-A577-4754-ABC8-31302CAF9674}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>